<commit_message>
added the function testing Assumption 1
</commit_message>
<xml_diff>
--- a/Data/Housing_data.xlsx
+++ b/Data/Housing_data.xlsx
@@ -8,14 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{353C7468-362C-4823-A547-FC731EED7D51}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4A690DF-E90B-468F-87E4-F87AEA74C6C0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{AB3678B5-2446-4328-882A-A72900DC8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction" sheetId="4" r:id="rId1"/>
     <sheet name="sale_counts" sheetId="1" r:id="rId2"/>
-    <sheet name="mean_sale_price" sheetId="2" r:id="rId3"/>
+    <sheet name="median_sale_price" sheetId="2" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -38,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2011" uniqueCount="225">
   <si>
     <t>Code</t>
   </si>
@@ -640,9 +640,6 @@
     <t>Wealden</t>
   </si>
   <si>
-    <t>:</t>
-  </si>
-  <si>
     <t>LA_Name</t>
   </si>
   <si>
@@ -650,9 +647,6 @@
   </si>
   <si>
     <t>Flats</t>
-  </si>
-  <si>
-    <t>c</t>
   </si>
   <si>
     <t>Source</t>
@@ -1685,82 +1679,82 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
-        <v>216</v>
+        <v>214</v>
       </c>
       <c r="B1" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A2" s="15" t="s">
-        <v>207</v>
+        <v>205</v>
       </c>
       <c r="B2" t="s">
-        <v>213</v>
+        <v>211</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="15" t="s">
-        <v>212</v>
+        <v>210</v>
       </c>
       <c r="B3" t="s">
-        <v>226</v>
+        <v>224</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A4" s="15" t="s">
-        <v>205</v>
+        <v>203</v>
       </c>
       <c r="B4" t="s">
-        <v>214</v>
+        <v>212</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A5" s="15" t="s">
-        <v>219</v>
+        <v>217</v>
       </c>
       <c r="B5" t="s">
-        <v>218</v>
+        <v>216</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A6" s="15" t="s">
-        <v>206</v>
+        <v>204</v>
       </c>
       <c r="B6" t="s">
-        <v>220</v>
+        <v>218</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A7" s="15" t="s">
-        <v>208</v>
+        <v>206</v>
       </c>
       <c r="B7" t="s">
-        <v>223</v>
+        <v>221</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A8" s="15" t="s">
-        <v>209</v>
+        <v>207</v>
       </c>
       <c r="B8" t="s">
-        <v>210</v>
+        <v>208</v>
       </c>
     </row>
     <row r="9" spans="1:2" ht="37" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="14" t="s">
-        <v>211</v>
+        <v>209</v>
       </c>
       <c r="B9" t="s">
-        <v>222</v>
+        <v>220</v>
       </c>
     </row>
     <row r="10" spans="1:2" ht="31" x14ac:dyDescent="0.35">
       <c r="A10" s="14" t="s">
-        <v>221</v>
+        <v>219</v>
       </c>
       <c r="B10" t="s">
-        <v>224</v>
+        <v>222</v>
       </c>
     </row>
   </sheetData>
@@ -1788,7 +1782,7 @@
   <dimension ref="A1:H491"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="E1" sqref="D1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -1801,13 +1795,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -1819,7 +1813,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -1914,10 +1908,10 @@
         <v>3887</v>
       </c>
       <c r="E5" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F5" s="10" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G5" s="10">
         <v>873</v>
@@ -14572,7 +14566,7 @@
   <dimension ref="A1:H491"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F53" sqref="F53"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14585,13 +14579,13 @@
         <v>0</v>
       </c>
       <c r="B1" s="6" t="s">
+        <v>200</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>201</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>202</v>
-      </c>
       <c r="D1" s="3" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="E1" s="3" t="s">
         <v>1</v>
@@ -14603,7 +14597,7 @@
         <v>3</v>
       </c>
       <c r="H1" s="4" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
@@ -14805,7 +14799,7 @@
         <v>85000</v>
       </c>
       <c r="F9" s="18">
-        <v>53000</v>
+        <v>-53000</v>
       </c>
       <c r="G9" s="18">
         <v>28000</v>
@@ -15946,10 +15940,10 @@
         <v>188750</v>
       </c>
       <c r="E53" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="F53" s="18" t="s">
-        <v>225</v>
+        <v>223</v>
       </c>
       <c r="G53" s="18">
         <v>223750</v>
@@ -16501,7 +16495,7 @@
         <v>23000</v>
       </c>
       <c r="H74" s="19" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -18156,7 +18150,7 @@
         <v>124000</v>
       </c>
       <c r="E138" s="18" t="s">
-        <v>204</v>
+        <v>223</v>
       </c>
       <c r="F138" s="18">
         <v>140000</v>
@@ -18390,13 +18384,13 @@
         <v>180000</v>
       </c>
       <c r="E147" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="F147" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="G147" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="H147" s="19">
         <v>162500</v>
@@ -20834,13 +20828,13 @@
         <v>225000</v>
       </c>
       <c r="E241" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="F241" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="G241" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="H241" s="19">
         <v>175000</v>
@@ -23281,7 +23275,7 @@
         <v>425000</v>
       </c>
       <c r="F335" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="G335" s="18">
         <v>301250</v>
@@ -25725,10 +25719,10 @@
         <v>400000</v>
       </c>
       <c r="F429" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="G429" s="18" t="s">
-        <v>200</v>
+        <v>223</v>
       </c>
       <c r="H429" s="19">
         <v>235000</v>

</xml_diff>

<commit_message>
adding function testing assumption 3
</commit_message>
<xml_diff>
--- a/Data/Housing_data.xlsx
+++ b/Data/Housing_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0D22FD37-98BA-432F-B84E-B64B7E077664}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71393AC3-7500-4DF1-998D-E313D45DBCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{AB3678B5-2446-4328-882A-A72900DC8DCC}"/>
   </bookViews>
@@ -27687,7 +27687,7 @@
   <dimension ref="A1:H51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J6" sqref="J6"/>
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -27734,8 +27734,8 @@
       <c r="D2" s="39">
         <v>52000</v>
       </c>
-      <c r="E2" s="40">
-        <v>92500</v>
+      <c r="E2" s="98">
+        <v>88000</v>
       </c>
       <c r="F2" s="42">
         <v>54000</v>

</xml_diff>

<commit_message>
Completed writing the code for testing assumptions
</commit_message>
<xml_diff>
--- a/Data/Housing_data.xlsx
+++ b/Data/Housing_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71393AC3-7500-4DF1-998D-E313D45DBCD0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987A52B6-0502-475C-B4C0-F27C667B4FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{AB3678B5-2446-4328-882A-A72900DC8DCC}"/>
   </bookViews>
@@ -1159,7 +1159,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="17">
+  <borders count="16">
     <border>
       <left/>
       <right/>
@@ -1334,15 +1334,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1407,7 +1398,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="100">
+  <cellXfs count="63">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1468,12 +1459,7 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
@@ -1481,159 +1467,69 @@
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="3" fontId="2" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{9F0C2C05-6E57-4D0C-BC6E-731B1C24F8F5}"/>
@@ -27684,7 +27580,7 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A095E8-09B6-4732-8565-763B56E913EC}">
-  <dimension ref="A1:H51"/>
+  <dimension ref="A1:I53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="E3" sqref="E3"/>
@@ -27695,7 +27591,7 @@
     <col min="2" max="2" width="24.3828125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" ht="24" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" ht="24" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -27721,8 +27617,8 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="38" t="s">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A2" s="35" t="s">
         <v>225</v>
       </c>
       <c r="B2" s="29" t="s">
@@ -27731,27 +27627,27 @@
       <c r="C2" s="28">
         <v>2000</v>
       </c>
-      <c r="D2" s="39">
+      <c r="D2" s="36">
         <v>52000</v>
       </c>
-      <c r="E2" s="98">
-        <v>88000</v>
-      </c>
-      <c r="F2" s="42">
+      <c r="E2" s="60">
+        <v>-88000</v>
+      </c>
+      <c r="F2" s="38">
         <v>54000</v>
       </c>
-      <c r="G2" s="44">
+      <c r="G2" s="39">
         <v>36000</v>
       </c>
-      <c r="H2" s="49">
+      <c r="H2" s="41">
         <v>36000</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="35" t="s">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A3" s="34" t="s">
         <v>227</v>
       </c>
-      <c r="B3" s="35" t="s">
+      <c r="B3" s="34" t="s">
         <v>228</v>
       </c>
       <c r="C3">
@@ -27760,24 +27656,24 @@
       <c r="D3" s="33">
         <v>56500</v>
       </c>
-      <c r="E3" s="40">
+      <c r="E3" s="37">
         <v>109000</v>
       </c>
-      <c r="F3" s="42">
+      <c r="F3" s="38">
         <v>59500</v>
       </c>
-      <c r="G3" s="44">
+      <c r="G3" s="39">
         <v>36050</v>
       </c>
-      <c r="H3" s="49">
+      <c r="H3" s="41">
         <v>53975</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" s="35" t="s">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A4" s="34" t="s">
         <v>229</v>
       </c>
-      <c r="B4" s="35" t="s">
+      <c r="B4" s="34" t="s">
         <v>230</v>
       </c>
       <c r="C4" s="28">
@@ -27786,24 +27682,24 @@
       <c r="D4" s="33">
         <v>56000</v>
       </c>
-      <c r="E4" s="40">
+      <c r="E4" s="37">
         <v>95000</v>
       </c>
-      <c r="F4" s="42">
+      <c r="F4" s="38">
         <v>54500</v>
       </c>
-      <c r="G4" s="44">
+      <c r="G4" s="39">
         <v>39000</v>
       </c>
-      <c r="H4" s="49">
+      <c r="H4" s="41">
         <v>52000</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" s="35" t="s">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A5" s="34" t="s">
         <v>231</v>
       </c>
-      <c r="B5" s="35" t="s">
+      <c r="B5" s="34" t="s">
         <v>232</v>
       </c>
       <c r="C5">
@@ -27812,24 +27708,24 @@
       <c r="D5" s="33">
         <v>61500</v>
       </c>
-      <c r="E5" s="40">
+      <c r="E5" s="37">
         <v>97000</v>
       </c>
-      <c r="F5" s="42">
+      <c r="F5" s="38">
         <v>55500</v>
       </c>
-      <c r="G5" s="44">
+      <c r="G5" s="39">
         <v>42950</v>
       </c>
-      <c r="H5" s="49">
+      <c r="H5" s="41">
         <v>43000</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="35" t="s">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A6" s="34" t="s">
         <v>233</v>
       </c>
-      <c r="B6" s="35" t="s">
+      <c r="B6" s="34" t="s">
         <v>234</v>
       </c>
       <c r="C6" s="28">
@@ -27838,24 +27734,24 @@
       <c r="D6" s="33">
         <v>67000</v>
       </c>
-      <c r="E6" s="40">
+      <c r="E6" s="37">
         <v>124000</v>
       </c>
-      <c r="F6" s="42">
+      <c r="F6" s="38">
         <v>65000</v>
       </c>
-      <c r="G6" s="44">
+      <c r="G6" s="39">
         <v>50000</v>
       </c>
-      <c r="H6" s="49">
+      <c r="H6" s="41">
         <v>47500</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" s="35" t="s">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A7" s="34" t="s">
         <v>235</v>
       </c>
-      <c r="B7" s="35" t="s">
+      <c r="B7" s="34" t="s">
         <v>236</v>
       </c>
       <c r="C7">
@@ -27864,24 +27760,24 @@
       <c r="D7" s="33">
         <v>86500</v>
       </c>
-      <c r="E7" s="40">
+      <c r="E7" s="37">
         <v>140000</v>
       </c>
-      <c r="F7" s="42">
+      <c r="F7" s="38">
         <v>85325</v>
       </c>
-      <c r="G7" s="44">
+      <c r="G7" s="39">
         <v>72000</v>
       </c>
-      <c r="H7" s="49">
+      <c r="H7" s="41">
         <v>59950</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A8" s="35" t="s">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A8" s="34" t="s">
         <v>237</v>
       </c>
-      <c r="B8" s="35" t="s">
+      <c r="B8" s="34" t="s">
         <v>238</v>
       </c>
       <c r="C8" s="28">
@@ -27890,1136 +27786,1172 @@
       <c r="D8" s="33">
         <v>138000</v>
       </c>
-      <c r="E8" s="40">
+      <c r="E8" s="37">
         <v>295000</v>
       </c>
-      <c r="F8" s="42">
+      <c r="F8" s="38">
         <v>165000</v>
       </c>
-      <c r="G8" s="44">
+      <c r="G8" s="39">
         <v>135000</v>
       </c>
-      <c r="H8" s="49">
+      <c r="H8" s="41">
         <v>120800</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" s="35" t="s">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A9" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B9" s="35" t="s">
+      <c r="B9" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C9">
+      <c r="C9" s="61">
         <v>2000</v>
       </c>
-      <c r="D9" s="33">
+      <c r="D9" s="60">
         <v>112000</v>
       </c>
-      <c r="E9" s="40">
+      <c r="E9" s="60">
         <v>193000</v>
       </c>
-      <c r="F9" s="42">
+      <c r="F9" s="60">
         <v>117751.5</v>
       </c>
-      <c r="G9" s="44">
+      <c r="G9" s="60">
         <v>89950</v>
       </c>
-      <c r="H9" s="49">
+      <c r="H9" s="60">
         <v>72500</v>
       </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" s="36" t="s">
+      <c r="I9" s="61"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A10" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B10" s="36" t="s">
+      <c r="B10" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C10" s="28">
+      <c r="C10" s="62">
         <v>2000</v>
       </c>
-      <c r="D10" s="33">
+      <c r="D10" s="60">
         <v>85000</v>
       </c>
-      <c r="E10" s="40">
+      <c r="E10" s="60">
         <v>137000</v>
       </c>
-      <c r="F10" s="42">
+      <c r="F10" s="60">
         <v>83100</v>
       </c>
-      <c r="G10" s="44">
+      <c r="G10" s="60">
         <v>68500</v>
       </c>
-      <c r="H10" s="49">
+      <c r="H10" s="60">
         <v>58950</v>
       </c>
-    </row>
-    <row r="11" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="37" t="s">
+      <c r="I10" s="61"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A11" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B11" s="37" t="s">
+      <c r="B11" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C11">
+      <c r="C11" s="61">
         <v>2000</v>
       </c>
-      <c r="D11" s="34">
+      <c r="D11" s="60">
         <v>56500</v>
       </c>
-      <c r="E11" s="41">
+      <c r="E11" s="60">
         <v>89500</v>
       </c>
-      <c r="F11" s="43">
+      <c r="F11" s="60">
         <v>54000</v>
       </c>
-      <c r="G11" s="45">
+      <c r="G11" s="60">
         <v>40000</v>
       </c>
-      <c r="H11" s="50">
+      <c r="H11" s="60">
         <v>49000</v>
       </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="46" t="s">
+      <c r="I11" s="61"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A12" s="58" t="s">
         <v>225</v>
       </c>
       <c r="B12" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C12">
+      <c r="C12" s="61">
         <v>2001</v>
       </c>
-      <c r="D12" s="51">
+      <c r="D12" s="60">
         <v>55000</v>
       </c>
-      <c r="E12" s="53">
+      <c r="E12" s="60">
         <v>99950</v>
       </c>
-      <c r="F12" s="55">
+      <c r="F12" s="60">
         <v>57500</v>
       </c>
-      <c r="G12" s="57">
+      <c r="G12" s="60">
         <v>37500</v>
       </c>
-      <c r="H12" s="62">
+      <c r="H12" s="60">
         <v>39000</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A13" s="46" t="s">
+      <c r="I12" s="61"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A13" s="40" t="s">
         <v>227</v>
       </c>
-      <c r="B13" s="46" t="s">
+      <c r="B13" s="40" t="s">
         <v>228</v>
       </c>
       <c r="C13">
         <v>2001</v>
       </c>
-      <c r="D13" s="51">
+      <c r="D13" s="42">
         <v>60000</v>
       </c>
-      <c r="E13" s="53">
+      <c r="E13" s="43">
         <v>119995</v>
       </c>
-      <c r="F13" s="55">
+      <c r="F13" s="44">
         <v>65000</v>
       </c>
-      <c r="G13" s="57">
+      <c r="G13" s="45">
         <v>38500</v>
       </c>
-      <c r="H13" s="62">
+      <c r="H13" s="47">
         <v>60000</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="46" t="s">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A14" s="40" t="s">
         <v>229</v>
       </c>
-      <c r="B14" s="46" t="s">
+      <c r="B14" s="40" t="s">
         <v>230</v>
       </c>
       <c r="C14">
         <v>2001</v>
       </c>
-      <c r="D14" s="51">
+      <c r="D14" s="42">
         <v>59950</v>
       </c>
-      <c r="E14" s="53">
+      <c r="E14" s="43">
         <v>105000</v>
       </c>
-      <c r="F14" s="55">
+      <c r="F14" s="44">
         <v>58950</v>
       </c>
-      <c r="G14" s="57">
+      <c r="G14" s="45">
         <v>40000</v>
       </c>
-      <c r="H14" s="62">
+      <c r="H14" s="47">
         <v>59950</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A15" s="46" t="s">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A15" s="40" t="s">
         <v>231</v>
       </c>
-      <c r="B15" s="46" t="s">
+      <c r="B15" s="40" t="s">
         <v>232</v>
       </c>
       <c r="C15">
         <v>2001</v>
       </c>
-      <c r="D15" s="51">
+      <c r="D15" s="42">
         <v>70000</v>
       </c>
-      <c r="E15" s="53">
+      <c r="E15" s="43">
         <v>112500</v>
       </c>
-      <c r="F15" s="55">
+      <c r="F15" s="44">
         <v>62000</v>
       </c>
-      <c r="G15" s="57">
+      <c r="G15" s="45">
         <v>48000</v>
       </c>
-      <c r="H15" s="62">
+      <c r="H15" s="47">
         <v>52000</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A16" s="46" t="s">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A16" s="40" t="s">
         <v>233</v>
       </c>
-      <c r="B16" s="46" t="s">
+      <c r="B16" s="40" t="s">
         <v>234</v>
       </c>
       <c r="C16">
         <v>2001</v>
       </c>
-      <c r="D16" s="51">
+      <c r="D16" s="42">
         <v>76000</v>
       </c>
-      <c r="E16" s="53">
+      <c r="E16" s="43">
         <v>138000</v>
       </c>
-      <c r="F16" s="55">
+      <c r="F16" s="44">
         <v>73000</v>
       </c>
-      <c r="G16" s="57">
+      <c r="G16" s="45">
         <v>56000</v>
       </c>
-      <c r="H16" s="62">
+      <c r="H16" s="47">
         <v>57000</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A17" s="46" t="s">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A17" s="40" t="s">
         <v>235</v>
       </c>
-      <c r="B17" s="46" t="s">
+      <c r="B17" s="40" t="s">
         <v>236</v>
       </c>
       <c r="C17">
         <v>2001</v>
       </c>
-      <c r="D17" s="51">
+      <c r="D17" s="42">
         <v>99995</v>
       </c>
-      <c r="E17" s="53">
+      <c r="E17" s="43">
         <v>155000</v>
       </c>
-      <c r="F17" s="55">
+      <c r="F17" s="44">
         <v>99995</v>
       </c>
-      <c r="G17" s="57">
+      <c r="G17" s="45">
         <v>82995</v>
       </c>
-      <c r="H17" s="62">
+      <c r="H17" s="47">
         <v>67000</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A18" s="46" t="s">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A18" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="B18" s="46" t="s">
+      <c r="B18" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="C18">
+      <c r="C18" s="61">
         <v>2001</v>
       </c>
-      <c r="D18" s="51">
+      <c r="D18" s="60">
         <v>155000</v>
       </c>
-      <c r="E18" s="53">
+      <c r="E18" s="60">
         <v>310000</v>
       </c>
-      <c r="F18" s="55">
+      <c r="F18" s="60">
         <v>182000</v>
       </c>
-      <c r="G18" s="57">
+      <c r="G18" s="60">
         <v>150000</v>
       </c>
-      <c r="H18" s="62">
+      <c r="H18" s="60">
         <v>136495</v>
       </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A19" s="46" t="s">
+      <c r="I18" s="61"/>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A19" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B19" s="46" t="s">
+      <c r="B19" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C19">
+      <c r="C19" s="61">
         <v>2001</v>
       </c>
-      <c r="D19" s="51">
+      <c r="D19" s="60">
         <v>126000</v>
       </c>
-      <c r="E19" s="53">
+      <c r="E19" s="60">
         <v>216500</v>
       </c>
-      <c r="F19" s="55">
+      <c r="F19" s="60">
         <v>130000</v>
       </c>
-      <c r="G19" s="57">
+      <c r="G19" s="60">
         <v>102500</v>
       </c>
-      <c r="H19" s="62">
+      <c r="H19" s="60">
         <v>84500</v>
       </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A20" s="47" t="s">
+      <c r="I19" s="61"/>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A20" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B20" s="47" t="s">
+      <c r="B20" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C20">
+      <c r="C20" s="61">
         <v>2001</v>
       </c>
-      <c r="D20" s="51">
+      <c r="D20" s="60">
         <v>96500</v>
       </c>
-      <c r="E20" s="53">
+      <c r="E20" s="60">
         <v>153000</v>
       </c>
-      <c r="F20" s="55">
+      <c r="F20" s="60">
         <v>94000</v>
       </c>
-      <c r="G20" s="57">
+      <c r="G20" s="60">
         <v>78000</v>
       </c>
-      <c r="H20" s="62">
+      <c r="H20" s="60">
         <v>69500</v>
       </c>
-    </row>
-    <row r="21" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A21" s="48" t="s">
+      <c r="I20" s="61"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B21" s="48" t="s">
+      <c r="B21" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C21">
+      <c r="C21" s="61">
         <v>2001</v>
       </c>
-      <c r="D21" s="52">
+      <c r="D21" s="60">
         <v>60000</v>
       </c>
-      <c r="E21" s="54">
+      <c r="E21" s="60">
         <v>97950</v>
       </c>
-      <c r="F21" s="56">
+      <c r="F21" s="60">
         <v>58000</v>
       </c>
-      <c r="G21" s="58">
+      <c r="G21" s="60">
         <v>43500</v>
       </c>
-      <c r="H21" s="63">
+      <c r="H21" s="60">
         <v>57000</v>
       </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A22" s="59" t="s">
+      <c r="I21" s="61"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="58" t="s">
         <v>225</v>
       </c>
       <c r="B22" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C22">
+      <c r="C22" s="61">
         <v>2002</v>
       </c>
-      <c r="D22" s="64">
+      <c r="D22" s="60">
         <v>60000</v>
       </c>
-      <c r="E22" s="66">
+      <c r="E22" s="60">
         <v>121950</v>
       </c>
-      <c r="F22" s="68">
+      <c r="F22" s="60">
         <v>66000</v>
       </c>
-      <c r="G22" s="70">
+      <c r="G22" s="60">
         <v>41950</v>
       </c>
-      <c r="H22" s="75">
+      <c r="H22" s="60">
         <v>47000</v>
       </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A23" s="59" t="s">
+      <c r="I22" s="61"/>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A23" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="B23" s="59" t="s">
+      <c r="B23" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C23">
+      <c r="C23" s="61">
         <v>2002</v>
       </c>
-      <c r="D23" s="64">
+      <c r="D23" s="60">
         <v>70000</v>
       </c>
-      <c r="E23" s="66">
+      <c r="E23" s="60">
         <v>140000</v>
       </c>
-      <c r="F23" s="68">
+      <c r="F23" s="60">
         <v>76950</v>
       </c>
-      <c r="G23" s="70">
+      <c r="G23" s="60">
         <v>43000</v>
       </c>
-      <c r="H23" s="75">
+      <c r="H23" s="60">
         <v>78950</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A24" s="59" t="s">
+      <c r="I23" s="61"/>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="46" t="s">
         <v>229</v>
       </c>
-      <c r="B24" s="59" t="s">
+      <c r="B24" s="46" t="s">
         <v>230</v>
       </c>
       <c r="C24">
         <v>2002</v>
       </c>
-      <c r="D24" s="64">
+      <c r="D24" s="48">
         <v>70000</v>
       </c>
-      <c r="E24" s="66">
+      <c r="E24" s="49">
         <v>129000</v>
       </c>
-      <c r="F24" s="68">
+      <c r="F24" s="50">
         <v>69950</v>
       </c>
-      <c r="G24" s="70">
+      <c r="G24" s="51">
         <v>46000</v>
       </c>
-      <c r="H24" s="75">
+      <c r="H24" s="53">
         <v>75500</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A25" s="59" t="s">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A25" s="46" t="s">
         <v>231</v>
       </c>
-      <c r="B25" s="59" t="s">
+      <c r="B25" s="46" t="s">
         <v>232</v>
       </c>
       <c r="C25">
         <v>2002</v>
       </c>
-      <c r="D25" s="64">
+      <c r="D25" s="48">
         <v>85000</v>
       </c>
-      <c r="E25" s="66">
+      <c r="E25" s="49">
         <v>135000</v>
       </c>
-      <c r="F25" s="68">
+      <c r="F25" s="50">
         <v>77000</v>
       </c>
-      <c r="G25" s="70">
+      <c r="G25" s="51">
         <v>59995</v>
       </c>
-      <c r="H25" s="75">
+      <c r="H25" s="53">
         <v>66000</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A26" s="59" t="s">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A26" s="46" t="s">
         <v>233</v>
       </c>
-      <c r="B26" s="59" t="s">
+      <c r="B26" s="46" t="s">
         <v>234</v>
       </c>
       <c r="C26">
         <v>2002</v>
       </c>
-      <c r="D26" s="64">
+      <c r="D26" s="48">
         <v>89950</v>
       </c>
-      <c r="E26" s="66">
+      <c r="E26" s="49">
         <v>162500</v>
       </c>
-      <c r="F26" s="68">
+      <c r="F26" s="50">
         <v>86500</v>
       </c>
-      <c r="G26" s="70">
+      <c r="G26" s="51">
         <v>67500</v>
       </c>
-      <c r="H26" s="75">
+      <c r="H26" s="53">
         <v>69500</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A27" s="59" t="s">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="46" t="s">
         <v>235</v>
       </c>
-      <c r="B27" s="59" t="s">
+      <c r="B27" s="46" t="s">
         <v>236</v>
       </c>
       <c r="C27">
         <v>2002</v>
       </c>
-      <c r="D27" s="64">
+      <c r="D27" s="48">
         <v>125000</v>
       </c>
-      <c r="E27" s="66">
+      <c r="E27" s="49">
         <v>185000</v>
       </c>
-      <c r="F27" s="68">
+      <c r="F27" s="50">
         <v>125000</v>
       </c>
-      <c r="G27" s="70">
+      <c r="G27" s="51">
         <v>104000</v>
       </c>
-      <c r="H27" s="75">
+      <c r="H27" s="53">
         <v>85950</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A28" s="59" t="s">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A28" s="46" t="s">
         <v>237</v>
       </c>
-      <c r="B28" s="59" t="s">
+      <c r="B28" s="46" t="s">
         <v>238</v>
       </c>
       <c r="C28">
         <v>2002</v>
       </c>
-      <c r="D28" s="64">
+      <c r="D28" s="48">
         <v>180457</v>
       </c>
-      <c r="E28" s="66">
+      <c r="E28" s="49">
         <v>352000</v>
       </c>
-      <c r="F28" s="68">
+      <c r="F28" s="50">
         <v>217000</v>
       </c>
-      <c r="G28" s="70">
+      <c r="G28" s="51">
         <v>180000</v>
       </c>
-      <c r="H28" s="75">
+      <c r="H28" s="53">
         <v>160000</v>
       </c>
     </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A29" s="59" t="s">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A29" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B29" s="59" t="s">
+      <c r="B29" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C29">
+      <c r="C29" s="61">
         <v>2002</v>
       </c>
-      <c r="D29" s="64">
+      <c r="D29" s="60">
         <v>148000</v>
       </c>
-      <c r="E29" s="66">
+      <c r="E29" s="60">
         <v>248000</v>
       </c>
-      <c r="F29" s="68">
+      <c r="F29" s="60">
         <v>153500</v>
       </c>
-      <c r="G29" s="70">
+      <c r="G29" s="60">
         <v>125000</v>
       </c>
-      <c r="H29" s="75">
+      <c r="H29" s="60">
         <v>104000</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A30" s="60" t="s">
+      <c r="I29" s="61"/>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A30" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B30" s="60" t="s">
+      <c r="B30" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C30">
+      <c r="C30" s="61">
         <v>2002</v>
       </c>
-      <c r="D30" s="64">
+      <c r="D30" s="60">
         <v>123000</v>
       </c>
-      <c r="E30" s="66">
+      <c r="E30" s="60">
         <v>185000</v>
       </c>
-      <c r="F30" s="68">
+      <c r="F30" s="60">
         <v>119000</v>
       </c>
-      <c r="G30" s="70">
+      <c r="G30" s="60">
         <v>97000</v>
       </c>
-      <c r="H30" s="75">
+      <c r="H30" s="60">
         <v>88000</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="61" t="s">
+      <c r="I30" s="61"/>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A31" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B31" s="61" t="s">
+      <c r="B31" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C31">
+      <c r="C31" s="61">
         <v>2002</v>
       </c>
-      <c r="D31" s="65">
+      <c r="D31" s="60">
         <v>71000</v>
       </c>
-      <c r="E31" s="67">
+      <c r="E31" s="60">
         <v>119950</v>
       </c>
-      <c r="F31" s="69">
+      <c r="F31" s="60">
         <v>67307.5</v>
       </c>
-      <c r="G31" s="71">
+      <c r="G31" s="60">
         <v>49950</v>
       </c>
-      <c r="H31" s="76">
+      <c r="H31" s="60">
         <v>69950</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A32" s="72" t="s">
+      <c r="I31" s="61"/>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A32" s="58" t="s">
         <v>225</v>
       </c>
       <c r="B32" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C32">
+      <c r="C32" s="61">
         <v>2003</v>
       </c>
-      <c r="D32" s="88">
+      <c r="D32" s="60">
         <v>77950</v>
       </c>
-      <c r="E32" s="83">
+      <c r="E32" s="60">
         <v>155000</v>
       </c>
-      <c r="F32" s="81">
+      <c r="F32" s="60">
         <v>85000</v>
       </c>
-      <c r="G32" s="79">
+      <c r="G32" s="60">
         <v>53000</v>
       </c>
-      <c r="H32" s="77">
+      <c r="H32" s="60">
         <v>63500</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A33" s="72" t="s">
+      <c r="I32" s="61"/>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A33" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="B33" s="72" t="s">
+      <c r="B33" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C33">
+      <c r="C33" s="61">
         <v>2003</v>
       </c>
-      <c r="D33" s="88">
+      <c r="D33" s="60">
         <v>85000</v>
       </c>
-      <c r="E33" s="83">
+      <c r="E33" s="60">
         <v>170950</v>
       </c>
-      <c r="F33" s="81">
+      <c r="F33" s="60">
         <v>94950</v>
       </c>
-      <c r="G33" s="79">
+      <c r="G33" s="60">
         <v>55000</v>
       </c>
-      <c r="H33" s="77">
+      <c r="H33" s="60">
         <v>93100</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A34" s="72" t="s">
+      <c r="I33" s="61"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A34" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="B34" s="72" t="s">
+      <c r="B34" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="C34">
+      <c r="C34" s="61">
         <v>2003</v>
       </c>
-      <c r="D34" s="88">
+      <c r="D34" s="60">
         <v>87950</v>
       </c>
-      <c r="E34" s="83">
+      <c r="E34" s="60">
         <v>161726</v>
       </c>
-      <c r="F34" s="81">
+      <c r="F34" s="60">
         <v>89500</v>
       </c>
-      <c r="G34" s="79">
+      <c r="G34" s="60">
         <v>59950</v>
       </c>
-      <c r="H34" s="77">
+      <c r="H34" s="60">
         <v>94000</v>
       </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A35" s="72" t="s">
+      <c r="I34" s="61"/>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A35" s="52" t="s">
         <v>231</v>
       </c>
-      <c r="B35" s="72" t="s">
+      <c r="B35" s="52" t="s">
         <v>232</v>
       </c>
       <c r="C35">
         <v>2003</v>
       </c>
-      <c r="D35" s="88">
+      <c r="D35" s="59">
         <v>107000</v>
       </c>
-      <c r="E35" s="83">
+      <c r="E35" s="57">
         <v>167000</v>
       </c>
-      <c r="F35" s="81">
+      <c r="F35" s="56">
         <v>97000</v>
       </c>
-      <c r="G35" s="79">
+      <c r="G35" s="55">
         <v>78000</v>
       </c>
-      <c r="H35" s="77">
+      <c r="H35" s="54">
         <v>87000</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A36" s="72" t="s">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A36" s="52" t="s">
         <v>233</v>
       </c>
-      <c r="B36" s="72" t="s">
+      <c r="B36" s="52" t="s">
         <v>234</v>
       </c>
       <c r="C36">
         <v>2003</v>
       </c>
-      <c r="D36" s="88">
+      <c r="D36" s="59">
         <v>110000</v>
       </c>
-      <c r="E36" s="83">
+      <c r="E36" s="57">
         <v>192450</v>
       </c>
-      <c r="F36" s="81">
+      <c r="F36" s="56">
         <v>108000</v>
       </c>
-      <c r="G36" s="79">
+      <c r="G36" s="55">
         <v>83500</v>
       </c>
-      <c r="H36" s="77">
+      <c r="H36" s="54">
         <v>88500</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A37" s="72" t="s">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A37" s="52" t="s">
         <v>235</v>
       </c>
-      <c r="B37" s="72" t="s">
+      <c r="B37" s="52" t="s">
         <v>236</v>
       </c>
       <c r="C37">
         <v>2003</v>
       </c>
-      <c r="D37" s="88">
+      <c r="D37" s="59">
         <v>145500</v>
       </c>
-      <c r="E37" s="83">
+      <c r="E37" s="57">
         <v>215000</v>
       </c>
-      <c r="F37" s="81">
+      <c r="F37" s="56">
         <v>148000</v>
       </c>
-      <c r="G37" s="79">
+      <c r="G37" s="55">
         <v>126000</v>
       </c>
-      <c r="H37" s="77">
+      <c r="H37" s="54">
         <v>105000</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A38" s="72" t="s">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A38" s="52" t="s">
         <v>237</v>
       </c>
-      <c r="B38" s="72" t="s">
+      <c r="B38" s="52" t="s">
         <v>238</v>
       </c>
       <c r="C38">
         <v>2003</v>
       </c>
-      <c r="D38" s="88">
+      <c r="D38" s="59">
         <v>200000</v>
       </c>
-      <c r="E38" s="83">
+      <c r="E38" s="57">
         <v>390000</v>
       </c>
-      <c r="F38" s="81">
+      <c r="F38" s="56">
         <v>245000</v>
       </c>
-      <c r="G38" s="79">
+      <c r="G38" s="55">
         <v>204525</v>
       </c>
-      <c r="H38" s="77">
+      <c r="H38" s="54">
         <v>173000</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A39" s="72" t="s">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A39" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B39" s="72" t="s">
+      <c r="B39" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C39">
+      <c r="C39" s="61">
         <v>2003</v>
       </c>
-      <c r="D39" s="88">
+      <c r="D39" s="60">
         <v>169950</v>
       </c>
-      <c r="E39" s="83">
+      <c r="E39" s="60">
         <v>279950</v>
       </c>
-      <c r="F39" s="81">
+      <c r="F39" s="60">
         <v>177500</v>
       </c>
-      <c r="G39" s="79">
+      <c r="G39" s="60">
         <v>144000</v>
       </c>
-      <c r="H39" s="77">
+      <c r="H39" s="60">
         <v>120000</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A40" s="73" t="s">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A40" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B40" s="73" t="s">
+      <c r="B40" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C40">
+      <c r="C40" s="61">
         <v>2003</v>
       </c>
-      <c r="D40" s="88">
+      <c r="D40" s="60">
         <v>145000</v>
       </c>
-      <c r="E40" s="83">
+      <c r="E40" s="60">
         <v>225000</v>
       </c>
-      <c r="F40" s="81">
+      <c r="F40" s="60">
         <v>141000</v>
       </c>
-      <c r="G40" s="79">
+      <c r="G40" s="60">
         <v>120000</v>
       </c>
-      <c r="H40" s="77">
+      <c r="H40" s="60">
         <v>108000</v>
       </c>
     </row>
-    <row r="41" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A41" s="74" t="s">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A41" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B41" s="74" t="s">
+      <c r="B41" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C41">
+      <c r="C41" s="61">
         <v>2003</v>
       </c>
-      <c r="D41" s="89">
+      <c r="D41" s="60">
         <v>88000</v>
       </c>
-      <c r="E41" s="84">
+      <c r="E41" s="60">
         <v>146972.5</v>
       </c>
-      <c r="F41" s="82">
+      <c r="F41" s="60">
         <v>85000</v>
       </c>
-      <c r="G41" s="80">
+      <c r="G41" s="60">
         <v>63000</v>
       </c>
-      <c r="H41" s="78">
+      <c r="H41" s="60">
         <v>85000</v>
       </c>
     </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A42" s="85" t="s">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A42" s="58" t="s">
         <v>225</v>
       </c>
       <c r="B42" s="29" t="s">
         <v>226</v>
       </c>
-      <c r="C42">
+      <c r="C42" s="61">
         <v>2004</v>
       </c>
-      <c r="D42" s="90">
+      <c r="D42" s="60">
         <v>96000</v>
       </c>
-      <c r="E42" s="92">
+      <c r="E42" s="60">
         <v>183500</v>
       </c>
-      <c r="F42" s="94">
+      <c r="F42" s="60">
         <v>110000</v>
       </c>
-      <c r="G42" s="96">
+      <c r="G42" s="60">
         <v>70000</v>
       </c>
-      <c r="H42" s="98">
+      <c r="H42" s="60">
         <v>82000</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A43" s="85" t="s">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A43" s="58" t="s">
         <v>227</v>
       </c>
-      <c r="B43" s="85" t="s">
+      <c r="B43" s="58" t="s">
         <v>228</v>
       </c>
-      <c r="C43">
+      <c r="C43" s="61">
         <v>2004</v>
       </c>
-      <c r="D43" s="90">
+      <c r="D43" s="60">
         <v>108000</v>
       </c>
-      <c r="E43" s="92">
+      <c r="E43" s="60">
         <v>200500</v>
       </c>
-      <c r="F43" s="94">
+      <c r="F43" s="60">
         <v>122000</v>
       </c>
-      <c r="G43" s="96">
+      <c r="G43" s="60">
         <v>72500</v>
       </c>
-      <c r="H43" s="98">
+      <c r="H43" s="60">
         <v>114000</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A44" s="85" t="s">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A44" s="58" t="s">
         <v>229</v>
       </c>
-      <c r="B44" s="85" t="s">
+      <c r="B44" s="58" t="s">
         <v>230</v>
       </c>
-      <c r="C44">
+      <c r="C44" s="61">
         <v>2004</v>
       </c>
-      <c r="D44" s="90">
+      <c r="D44" s="60">
         <v>110000</v>
       </c>
-      <c r="E44" s="92">
+      <c r="E44" s="60">
         <v>189950</v>
       </c>
-      <c r="F44" s="94">
+      <c r="F44" s="60">
         <v>115000</v>
       </c>
-      <c r="G44" s="96">
+      <c r="G44" s="60">
         <v>77000</v>
       </c>
-      <c r="H44" s="98">
+      <c r="H44" s="60">
         <v>115000</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A45" s="85" t="s">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A45" s="58" t="s">
         <v>231</v>
       </c>
-      <c r="B45" s="85" t="s">
+      <c r="B45" s="58" t="s">
         <v>232</v>
       </c>
-      <c r="C45">
+      <c r="C45" s="61">
         <v>2004</v>
       </c>
-      <c r="D45" s="90">
+      <c r="D45" s="60">
         <v>126355</v>
       </c>
-      <c r="E45" s="92">
+      <c r="E45" s="60">
         <v>187000</v>
       </c>
-      <c r="F45" s="94">
+      <c r="F45" s="60">
         <v>118000</v>
       </c>
-      <c r="G45" s="96">
+      <c r="G45" s="60">
         <v>94000</v>
       </c>
-      <c r="H45" s="98">
+      <c r="H45" s="60">
         <v>102000</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A46" s="85" t="s">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A46" s="58" t="s">
         <v>233</v>
       </c>
-      <c r="B46" s="85" t="s">
+      <c r="B46" s="58" t="s">
         <v>234</v>
       </c>
-      <c r="C46">
+      <c r="C46" s="61">
         <v>2004</v>
       </c>
-      <c r="D46" s="90">
+      <c r="D46" s="60">
         <v>128500</v>
       </c>
-      <c r="E46" s="92">
+      <c r="E46" s="60">
         <v>220000</v>
       </c>
-      <c r="F46" s="94">
+      <c r="F46" s="60">
         <v>127500</v>
       </c>
-      <c r="G46" s="96">
+      <c r="G46" s="60">
         <v>100000</v>
       </c>
-      <c r="H46" s="98">
+      <c r="H46" s="60">
         <v>105000</v>
       </c>
     </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A47" s="85" t="s">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A47" s="58" t="s">
         <v>235</v>
       </c>
-      <c r="B47" s="85" t="s">
+      <c r="B47" s="58" t="s">
         <v>236</v>
       </c>
-      <c r="C47">
+      <c r="C47" s="61">
         <v>2004</v>
       </c>
-      <c r="D47" s="90">
+      <c r="D47" s="60">
         <v>164000</v>
       </c>
-      <c r="E47" s="92">
+      <c r="E47" s="60">
         <v>235000</v>
       </c>
-      <c r="F47" s="94">
+      <c r="F47" s="60">
         <v>165000</v>
       </c>
-      <c r="G47" s="96">
+      <c r="G47" s="60">
         <v>142000</v>
       </c>
-      <c r="H47" s="98">
+      <c r="H47" s="60">
         <v>120000</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A48" s="85" t="s">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A48" s="58" t="s">
         <v>237</v>
       </c>
-      <c r="B48" s="85" t="s">
+      <c r="B48" s="58" t="s">
         <v>238</v>
       </c>
-      <c r="C48">
+      <c r="C48" s="61">
         <v>2004</v>
       </c>
-      <c r="D48" s="90">
+      <c r="D48" s="60">
         <v>220000</v>
       </c>
-      <c r="E48" s="92">
+      <c r="E48" s="60">
         <v>430000</v>
       </c>
-      <c r="F48" s="94">
+      <c r="F48" s="60">
         <v>250000</v>
       </c>
-      <c r="G48" s="96">
+      <c r="G48" s="60">
         <v>225000</v>
       </c>
-      <c r="H48" s="98">
+      <c r="H48" s="60">
         <v>191000</v>
       </c>
     </row>
     <row r="49" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A49" s="85" t="s">
+      <c r="A49" s="58" t="s">
         <v>239</v>
       </c>
-      <c r="B49" s="85" t="s">
+      <c r="B49" s="58" t="s">
         <v>240</v>
       </c>
-      <c r="C49">
+      <c r="C49" s="61">
         <v>2004</v>
       </c>
-      <c r="D49" s="90">
+      <c r="D49" s="60">
         <v>185000</v>
       </c>
-      <c r="E49" s="92">
+      <c r="E49" s="60">
         <v>300000</v>
       </c>
-      <c r="F49" s="94">
+      <c r="F49" s="60">
         <v>192000</v>
       </c>
-      <c r="G49" s="96">
+      <c r="G49" s="60">
         <v>158500</v>
       </c>
-      <c r="H49" s="98">
+      <c r="H49" s="60">
         <v>134950</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A50" s="86" t="s">
+      <c r="A50" s="58" t="s">
         <v>241</v>
       </c>
-      <c r="B50" s="86" t="s">
+      <c r="B50" s="58" t="s">
         <v>242</v>
       </c>
-      <c r="C50">
+      <c r="C50" s="61">
         <v>2004</v>
       </c>
-      <c r="D50" s="90">
+      <c r="D50" s="60">
         <v>164950</v>
       </c>
-      <c r="E50" s="92">
+      <c r="E50" s="60">
         <v>247000</v>
       </c>
-      <c r="F50" s="94">
+      <c r="F50" s="60">
         <v>160000</v>
       </c>
-      <c r="G50" s="96">
+      <c r="G50" s="60">
         <v>137500</v>
       </c>
-      <c r="H50" s="98">
+      <c r="H50" s="60">
         <v>124950</v>
       </c>
     </row>
-    <row r="51" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A51" s="87" t="s">
+    <row r="51" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A51" s="58" t="s">
         <v>243</v>
       </c>
-      <c r="B51" s="87" t="s">
+      <c r="B51" s="58" t="s">
         <v>244</v>
       </c>
-      <c r="C51">
+      <c r="C51" s="61">
         <v>2004</v>
       </c>
-      <c r="D51" s="91">
+      <c r="D51" s="60">
         <v>115000</v>
       </c>
-      <c r="E51" s="93">
+      <c r="E51" s="60">
         <v>177000</v>
       </c>
-      <c r="F51" s="95">
+      <c r="F51" s="60">
         <v>111950</v>
       </c>
-      <c r="G51" s="97">
+      <c r="G51" s="60">
         <v>83000</v>
       </c>
-      <c r="H51" s="99">
+      <c r="H51" s="60">
         <v>110000</v>
       </c>
+    </row>
+    <row r="52" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A52" s="61"/>
+      <c r="B52" s="61"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="61"/>
+      <c r="E52" s="61"/>
+      <c r="F52" s="61"/>
+      <c r="G52" s="61"/>
+      <c r="H52" s="61"/>
+    </row>
+    <row r="53" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A53" s="61"/>
+      <c r="B53" s="61"/>
+      <c r="C53" s="61"/>
+      <c r="D53" s="61"/>
+      <c r="E53" s="61"/>
+      <c r="F53" s="61"/>
+      <c r="G53" s="61"/>
+      <c r="H53" s="61"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
changed the data sheet name to match the data with the screenshot on example_script.py
</commit_message>
<xml_diff>
--- a/Data/Housing_data.xlsx
+++ b/Data/Housing_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_demo\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{987A52B6-0502-475C-B4C0-F27C667B4FF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE7BAA17-2056-473B-9016-E8059ACCD00E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{AB3678B5-2446-4328-882A-A72900DC8DCC}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="2" xr2:uid="{AB3678B5-2446-4328-882A-A72900DC8DCC}"/>
   </bookViews>
   <sheets>
     <sheet name="introduction" sheetId="4" r:id="rId1"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2119" uniqueCount="245">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2118" uniqueCount="245">
   <si>
     <t>Code</t>
   </si>
@@ -972,7 +972,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1155,6 +1155,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1398,7 +1404,7 @@
     <xf numFmtId="0" fontId="22" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="63">
+  <cellXfs count="68">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1"/>
@@ -1530,6 +1536,17 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="34" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="3" fontId="20" fillId="34" borderId="11" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="34" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="3" fontId="20" fillId="34" borderId="10" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="55">
     <cellStyle name="20% - Accent1 2" xfId="2" xr:uid="{9F0C2C05-6E57-4D0C-BC6E-731B1C24F8F5}"/>
@@ -14798,8 +14815,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D85B4453-11F1-496E-AA5E-A13E57016F5E}">
   <dimension ref="A1:H491"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:H1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
@@ -14833,30 +14850,30 @@
         <v>202</v>
       </c>
     </row>
-    <row r="2" spans="1:8" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A2" s="22" t="s">
+    <row r="2" spans="1:8" s="67" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="63" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="22" t="s">
+      <c r="B2" s="63" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="22">
+      <c r="C2" s="63">
         <v>2000</v>
       </c>
-      <c r="D2" s="23">
-        <v>47000</v>
-      </c>
-      <c r="E2" s="24">
+      <c r="D2" s="64">
+        <v>-47000</v>
+      </c>
+      <c r="E2" s="65">
         <v>87995</v>
       </c>
-      <c r="F2" s="24">
+      <c r="F2" s="65">
         <v>52500</v>
       </c>
-      <c r="G2" s="24">
+      <c r="G2" s="65">
         <v>25000</v>
       </c>
-      <c r="H2" s="25">
-        <v>31475</v>
+      <c r="H2" s="66">
+        <v>-31475</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
@@ -15064,7 +15081,7 @@
         <v>38000</v>
       </c>
       <c r="H10" s="19">
-        <v>36375</v>
+        <v>-36375</v>
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
@@ -16727,8 +16744,8 @@
       <c r="G74" s="18">
         <v>23000</v>
       </c>
-      <c r="H74" s="19" t="s">
-        <v>223</v>
+      <c r="H74" s="19">
+        <v>0</v>
       </c>
     </row>
     <row r="75" spans="1:8" x14ac:dyDescent="0.35">
@@ -27582,8 +27599,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F3A095E8-09B6-4732-8565-763B56E913EC}">
   <dimension ref="A1:I53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D1" sqref="D1:D1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>